<commit_message>
added composite layering ex prelim work to FEA
</commit_message>
<xml_diff>
--- a/Analysis/FEA/Full_Tank_Analysis/FEA_Full_Tank_Model_Analysis_Workbook.xlsx
+++ b/Analysis/FEA/Full_Tank_Analysis/FEA_Full_Tank_Model_Analysis_Workbook.xlsx
@@ -14,6 +14,7 @@
   <sheets>
     <sheet name="Plasticity Modeling" sheetId="1" r:id="rId1"/>
     <sheet name="Material Properties" sheetId="2" r:id="rId2"/>
+    <sheet name="Additional ABAQUS Resources" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Stress/Strain Data from webplotdigitizer</t>
   </si>
@@ -67,6 +68,24 @@
   </si>
   <si>
     <t>Using 0.031 in-sheet liner design</t>
+  </si>
+  <si>
+    <t>Resources</t>
+  </si>
+  <si>
+    <t>Also see Resources folder under FEA on Git</t>
+  </si>
+  <si>
+    <t>Composite layer tutorial</t>
+  </si>
+  <si>
+    <t>https://sites.google.com/site/abaqus2010/tutorial_1</t>
+  </si>
+  <si>
+    <t>CF missing material properties (estimations, props we don’t have for ESL/LW analysis)</t>
+  </si>
+  <si>
+    <t>http://www.performance-composites.com/carbonfibre/mechanicalproperties_2.asp</t>
   </si>
 </sst>
 </file>
@@ -112,10 +131,10 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -633,7 +652,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -756,7 +774,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -917,7 +934,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1297,7 +1313,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1420,7 +1435,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3050,12 +3064,12 @@
       <c r="D1" s="3"/>
     </row>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
@@ -3642,18 +3656,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="1" t="s">
         <v>10</v>
       </c>
     </row>
@@ -3669,7 +3683,7 @@
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>7</v>
       </c>
     </row>
@@ -3679,7 +3693,7 @@
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="1" t="s">
         <v>8</v>
       </c>
     </row>
@@ -3692,4 +3706,88 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:J8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B7:J7"/>
+    <mergeCell ref="B8:J8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated FEA workbook, added additional FEA resources
</commit_message>
<xml_diff>
--- a/Analysis/FEA/Full_Tank_Analysis/FEA_Full_Tank_Model_Analysis_Workbook.xlsx
+++ b/Analysis/FEA/Full_Tank_Analysis/FEA_Full_Tank_Model_Analysis_Workbook.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\khensu\Home01\nab2\Desktop\FEA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\khensu\Home01\nab2\Desktop\FEA\Full_Tank_Model\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22170" windowHeight="10005" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22170" windowHeight="10005" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Plasticity Modeling" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Stress/Strain Data from webplotdigitizer</t>
   </si>
@@ -87,12 +87,18 @@
   <si>
     <t>http://www.performance-composites.com/carbonfibre/mechanicalproperties_2.asp</t>
   </si>
+  <si>
+    <t>Notes:</t>
+  </si>
+  <si>
+    <t>Turns out this tut may not be that useful aside from where to assign material properties</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -104,6 +110,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -126,10 +140,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -138,8 +153,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3645,7 +3664,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
@@ -3710,10 +3729,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:J8"/>
+  <dimension ref="B2:S8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3721,12 +3740,12 @@
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>15</v>
       </c>
@@ -3734,8 +3753,11 @@
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
-    </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K3" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>16</v>
       </c>
@@ -3743,8 +3765,8 @@
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B5" s="2" t="s">
+    <row r="5" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B5" s="4" t="s">
         <v>17</v>
       </c>
       <c r="C5" s="2"/>
@@ -3752,8 +3774,19 @@
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
-    </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="2"/>
+      <c r="S5" s="2"/>
+    </row>
+    <row r="7" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>18</v>
       </c>
@@ -3766,7 +3799,7 @@
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>19</v>
       </c>
@@ -3780,14 +3813,18 @@
       <c r="J8" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="K5:S5"/>
     <mergeCell ref="B3:F3"/>
     <mergeCell ref="B4:E4"/>
     <mergeCell ref="B5:G5"/>
     <mergeCell ref="B7:J7"/>
     <mergeCell ref="B8:J8"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B5" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>